<commit_message>
Updates to dashboard and the burndowncharts
</commit_message>
<xml_diff>
--- a/Burndown Chart/Burndown Charts.xlsx
+++ b/Burndown Chart/Burndown Charts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f00c811aa47a02b7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\OTS-Courier-Services\Burndown Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="8595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10130" windowHeight="8600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Hours Spent</t>
   </si>
@@ -126,6 +126,54 @@
   </si>
   <si>
     <t>Story 18</t>
+  </si>
+  <si>
+    <t>Story 19</t>
+  </si>
+  <si>
+    <t>Story 20</t>
+  </si>
+  <si>
+    <t>Story 16</t>
+  </si>
+  <si>
+    <t>Story 17</t>
+  </si>
+  <si>
+    <t>Story 2</t>
+  </si>
+  <si>
+    <t>Story 3</t>
+  </si>
+  <si>
+    <t>Day 21</t>
+  </si>
+  <si>
+    <t>Day 22</t>
+  </si>
+  <si>
+    <t>Day 23</t>
+  </si>
+  <si>
+    <t>Day 24</t>
+  </si>
+  <si>
+    <t>Day 25</t>
+  </si>
+  <si>
+    <t>Day 26</t>
+  </si>
+  <si>
+    <t>Day 27</t>
+  </si>
+  <si>
+    <t>Day 28</t>
+  </si>
+  <si>
+    <t>Day 29</t>
+  </si>
+  <si>
+    <t>Day 30</t>
   </si>
 </sst>
 </file>
@@ -1197,6 +1245,524 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> Chart Sprint 3</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$C$11:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E658-4BE6-A1B1-A15D033F44A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 3'!$C$12:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>52.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.800000000000011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.20000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.400000000000009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.8000000000000087</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E658-4BE6-A1B1-A15D033F44A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="459391488"/>
+        <c:axId val="459390176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="459391488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Days</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> within Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="459390176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="459390176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Hours of Work</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="459391488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1277,6 +1843,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1794,6 +2400,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2358,6 +3480,41 @@
       <xdr:colOff>552450</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>168275</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2678,25 +3835,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="A3:M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -2728,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2767,16 +3924,16 @@
         <v>3</v>
       </c>
       <c r="M5">
-        <f>SUM(C5:L5)</f>
+        <f t="shared" ref="M5:M10" si="0">SUM(C5:L5)</f>
         <v>14.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B10" si="0">C6+D6+E6+F6+G6+H6+I6+J6+K6+L6</f>
+        <f t="shared" ref="B6:B10" si="1">C6+D6+E6+F6+G6+H6+I6+J6+K6+L6</f>
         <v>7.5</v>
       </c>
       <c r="C6">
@@ -2810,183 +3967,183 @@
         <v>2</v>
       </c>
       <c r="M6">
-        <f>SUM(C6:L6)</f>
+        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1.5</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>1.5</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <f>SUM(C7:L7)</f>
-        <v>6.5</v>
-      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>2.5</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>2.5</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
-      <c r="L8">
-        <v>2</v>
-      </c>
-      <c r="M8">
-        <f>SUM(C8:L8)</f>
-        <v>6.5</v>
-      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <f>SUM(C9:L9)</f>
-        <v>7</v>
-      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <f>SUM(C10:L10)</f>
-        <v>9</v>
-      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2999,43 +4156,43 @@
         <v>51</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:L11" si="1">C11-SUM(D5:D10)</f>
+        <f t="shared" ref="D11:L11" si="2">C11-SUM(D5:D10)</f>
         <v>47</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.5</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3098,12 +4255,12 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>2</v>
       </c>
@@ -3135,7 +4292,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3178,7 +4335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -3221,7 +4378,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3264,7 +4421,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -3307,7 +4464,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3316,47 +4473,47 @@
         <v>29</v>
       </c>
       <c r="C6">
-        <f>B6-SUM(C2:C5)</f>
+        <f t="shared" ref="C6:L6" si="1">B6-SUM(C2:C5)</f>
         <v>29</v>
       </c>
       <c r="D6">
-        <f>C6-SUM(D2:D5)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="E6">
-        <f>D6-SUM(E2:E5)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="F6">
-        <f>E6-SUM(F2:F5)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G6">
-        <f>F6-SUM(G2:G5)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="H6">
-        <f>G6-SUM(H2:H5)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I6">
-        <f>H6-SUM(I2:I5)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J6">
-        <f>I6-SUM(J2:J5)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K6">
-        <f>J6-SUM(K2:K5)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L6">
-        <f>K6-SUM(L2:L5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -3412,15 +4569,427 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5</f>
+        <v>7.5</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>0.5</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M10" si="0">SUM(C5:L5)</f>
+        <v>7.5</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:B10" si="1">C6+D6+E6+F6+G6+H6+I6+J6+K6+L6</f>
+        <v>5.5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1.5</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="P6">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B5:B10)</f>
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <f>B11-SUM(C5:C10)</f>
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:L11" si="2">C11-SUM(D5:D10)</f>
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>58</v>
+      </c>
+      <c r="C12">
+        <f>B12-(B12/10)</f>
+        <v>52.2</v>
+      </c>
+      <c r="D12">
+        <f>C12-(B12/10)</f>
+        <v>46.400000000000006</v>
+      </c>
+      <c r="E12">
+        <f>D12-(B12/10)</f>
+        <v>40.600000000000009</v>
+      </c>
+      <c r="F12">
+        <f>E12-(B12/10)</f>
+        <v>34.800000000000011</v>
+      </c>
+      <c r="G12">
+        <f>F12-(B12/10)</f>
+        <v>29.000000000000011</v>
+      </c>
+      <c r="H12">
+        <f>G12-(B12/10)</f>
+        <v>23.20000000000001</v>
+      </c>
+      <c r="I12">
+        <f>H12-(B12/10)</f>
+        <v>17.400000000000009</v>
+      </c>
+      <c r="J12">
+        <f>I12-(B12/10)</f>
+        <v>11.600000000000009</v>
+      </c>
+      <c r="K12" s="2">
+        <f>J12-(B12/10)</f>
+        <v>5.8000000000000087</v>
+      </c>
+      <c r="L12">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3430,7 +4999,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Sprint 4 burndown Chart Updates
</commit_message>
<xml_diff>
--- a/Burndown Chart/Burndown Charts.xlsx
+++ b/Burndown Chart/Burndown Charts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10130" windowHeight="8600" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10130" windowHeight="8600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>Hours Spent</t>
   </si>
@@ -174,6 +174,63 @@
   </si>
   <si>
     <t>Day 30</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Story 6</t>
+  </si>
+  <si>
+    <t>Story 7</t>
+  </si>
+  <si>
+    <t>Veronica</t>
+  </si>
+  <si>
+    <t>Story 21</t>
+  </si>
+  <si>
+    <t>Hayden</t>
+  </si>
+  <si>
+    <t>Reeve</t>
+  </si>
+  <si>
+    <t>Modification</t>
+  </si>
+  <si>
+    <t>Day 31</t>
+  </si>
+  <si>
+    <t>Day 32</t>
+  </si>
+  <si>
+    <t>Day 33</t>
+  </si>
+  <si>
+    <t>Day 34</t>
+  </si>
+  <si>
+    <t>Day 35</t>
+  </si>
+  <si>
+    <t>Day 36</t>
+  </si>
+  <si>
+    <t>Day 37</t>
+  </si>
+  <si>
+    <t>Day 38</t>
+  </si>
+  <si>
+    <t>Day 39</t>
+  </si>
+  <si>
+    <t>Day 40</t>
+  </si>
+  <si>
+    <t>Matthew</t>
   </si>
 </sst>
 </file>
@@ -1763,6 +1820,372 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$C$9:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7AF1-41B2-BA39-177A1EB162D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$C$10:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>52.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.800000000000011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.20000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.400000000000009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.8000000000000087</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7AF1-41B2-BA39-177A1EB162D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="324928104"/>
+        <c:axId val="324928760"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="324928104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="324928760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="324928760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="324928104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1883,6 +2306,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2916,6 +3379,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3514,6 +4493,41 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>168275</xdr:colOff>
       <xdr:row>31</xdr:row>
+      <xdr:rowOff>98425</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>34925</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>117475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>339725</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>98425</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4571,8 +5585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4995,12 +6009,380 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4</f>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M8" si="0">SUM(C4:L4)</f>
+        <v>4</v>
+      </c>
+      <c r="P4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B8" si="1">C5+D5+E5+F5+G5+H5+I5+J5+K5+L5</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="P8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B4:B8)</f>
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:L9" si="2">B9-SUM(C4:C8)</f>
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>58</v>
+      </c>
+      <c r="C10">
+        <f>B10-(B10/10)</f>
+        <v>52.2</v>
+      </c>
+      <c r="D10">
+        <f>C10-(B10/10)</f>
+        <v>46.400000000000006</v>
+      </c>
+      <c r="E10">
+        <f>D10-(B10/10)</f>
+        <v>40.600000000000009</v>
+      </c>
+      <c r="F10">
+        <f>E10-(B10/10)</f>
+        <v>34.800000000000011</v>
+      </c>
+      <c r="G10">
+        <f>F10-(B10/10)</f>
+        <v>29.000000000000011</v>
+      </c>
+      <c r="H10">
+        <f>G10-(B10/10)</f>
+        <v>23.20000000000001</v>
+      </c>
+      <c r="I10">
+        <f>H10-(B10/10)</f>
+        <v>17.400000000000009</v>
+      </c>
+      <c r="J10">
+        <f>I10-(B10/10)</f>
+        <v>11.600000000000009</v>
+      </c>
+      <c r="K10" s="2">
+        <f>J10-(B10/10)</f>
+        <v>5.8000000000000087</v>
+      </c>
+      <c r="L10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed phoen orders booking page. ANd updated burndown chart
</commit_message>
<xml_diff>
--- a/Burndown Chart/Burndown Charts.xlsx
+++ b/Burndown Chart/Burndown Charts.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Veronica\Documents\OTS-Courier-Services\Burndown Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Magin\Documents\OTS-Courier-Services\Burndown Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="8" r:id="rId5"/>
+    <sheet name="Release 1" sheetId="5" r:id="rId6"/>
+    <sheet name="Release 2" sheetId="6" r:id="rId7"/>
+    <sheet name="Assigned Stories" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="223">
   <si>
     <t>Hours Spent</t>
   </si>
@@ -231,16 +235,478 @@
   </si>
   <si>
     <t>Matthew</t>
+  </si>
+  <si>
+    <t>Story Name</t>
+  </si>
+  <si>
+    <t>Task No</t>
+  </si>
+  <si>
+    <t>Task Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Estimated Hours</t>
+  </si>
+  <si>
+    <t>Effort Hours Remaining</t>
+  </si>
+  <si>
+    <t>Create a home page (customers view of website)</t>
+  </si>
+  <si>
+    <t>Write test cases</t>
+  </si>
+  <si>
+    <t>Create login system for customers (connects to database)</t>
+  </si>
+  <si>
+    <t>Create profile / shipping management page</t>
+  </si>
+  <si>
+    <t>Create table in the database to store pickup requests</t>
+  </si>
+  <si>
+    <t>Create book shipment form</t>
+  </si>
+  <si>
+    <t>Write code to connect and submit to the database (pickup request table)</t>
+  </si>
+  <si>
+    <t>Create page to show all pending shipments</t>
+  </si>
+  <si>
+    <t>Verify story is complete (acceptance criteria test)</t>
+  </si>
+  <si>
+    <t>T001</t>
+  </si>
+  <si>
+    <t>T002</t>
+  </si>
+  <si>
+    <t>T003</t>
+  </si>
+  <si>
+    <t>T004</t>
+  </si>
+  <si>
+    <t>T005</t>
+  </si>
+  <si>
+    <t>T006</t>
+  </si>
+  <si>
+    <t>T007</t>
+  </si>
+  <si>
+    <t>T008</t>
+  </si>
+  <si>
+    <t>T009</t>
+  </si>
+  <si>
+    <t>T010</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Time Taken</t>
+  </si>
+  <si>
+    <t>Create a tracking page (customers view of website)</t>
+  </si>
+  <si>
+    <t>Connecting to the database and selecting the unique tracking number.</t>
+  </si>
+  <si>
+    <t>Create page outputting the results of the tracking number in a visually appealing tabular format.</t>
+  </si>
+  <si>
+    <t>T011</t>
+  </si>
+  <si>
+    <t>T012</t>
+  </si>
+  <si>
+    <t>T013</t>
+  </si>
+  <si>
+    <t>T014</t>
+  </si>
+  <si>
+    <t>T015</t>
+  </si>
+  <si>
+    <t>T016</t>
+  </si>
+  <si>
+    <t>T017</t>
+  </si>
+  <si>
+    <t>T018</t>
+  </si>
+  <si>
+    <t>T019</t>
+  </si>
+  <si>
+    <t>T020</t>
+  </si>
+  <si>
+    <t>T021</t>
+  </si>
+  <si>
+    <t>T022</t>
+  </si>
+  <si>
+    <t>T023</t>
+  </si>
+  <si>
+    <t>T024</t>
+  </si>
+  <si>
+    <t>T025</t>
+  </si>
+  <si>
+    <t>T026</t>
+  </si>
+  <si>
+    <t>T027</t>
+  </si>
+  <si>
+    <t>T028</t>
+  </si>
+  <si>
+    <t>T029</t>
+  </si>
+  <si>
+    <t>T030</t>
+  </si>
+  <si>
+    <t>T031</t>
+  </si>
+  <si>
+    <t>Create the pdf template for the consignment note.</t>
+  </si>
+  <si>
+    <t>Write test cases.</t>
+  </si>
+  <si>
+    <t>Connect to database and select relevant information for the consignment note.</t>
+  </si>
+  <si>
+    <t>Generate a printable copy of the consignment note.</t>
+  </si>
+  <si>
+    <t>Write code to save the consignment note to the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create the estimate shipping webpage. </t>
+  </si>
+  <si>
+    <t>Write code (formula) to calculate the shipping cost based off the information given in the form.</t>
+  </si>
+  <si>
+    <t>Create page to output the results of the calculation</t>
+  </si>
+  <si>
+    <t>Verify story is complete (acceptance criteria test).</t>
+  </si>
+  <si>
+    <t>Create the pdf template for the tax invoice.</t>
+  </si>
+  <si>
+    <t>Connect to database and select relevant information for the tax invoice.</t>
+  </si>
+  <si>
+    <t>Generate a printable copy of the tax invoice.</t>
+  </si>
+  <si>
+    <t>Write code to email a pdf copy of the invoice.</t>
+  </si>
+  <si>
+    <t>Write code to save the tax invoice to the database</t>
+  </si>
+  <si>
+    <t>T032</t>
+  </si>
+  <si>
+    <t>T033</t>
+  </si>
+  <si>
+    <t>T034</t>
+  </si>
+  <si>
+    <t>T035</t>
+  </si>
+  <si>
+    <t>T036</t>
+  </si>
+  <si>
+    <t>T037</t>
+  </si>
+  <si>
+    <t>T038</t>
+  </si>
+  <si>
+    <t>T039</t>
+  </si>
+  <si>
+    <t>T040</t>
+  </si>
+  <si>
+    <t>Create registration page (where users registers).</t>
+  </si>
+  <si>
+    <t>Write code to submit the registration information to the database</t>
+  </si>
+  <si>
+    <t>Create a personal profile page and write code to retrieve user details from the database.</t>
+  </si>
+  <si>
+    <t>Write code to retrieve the user information from the database and output it to the “make a booking” page.</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>T041</t>
+  </si>
+  <si>
+    <t>T042</t>
+  </si>
+  <si>
+    <t>T043</t>
+  </si>
+  <si>
+    <t>T044</t>
+  </si>
+  <si>
+    <t>T045</t>
+  </si>
+  <si>
+    <t>T046</t>
+  </si>
+  <si>
+    <t>T047</t>
+  </si>
+  <si>
+    <t>T048</t>
+  </si>
+  <si>
+    <t>T049</t>
+  </si>
+  <si>
+    <t>T050</t>
+  </si>
+  <si>
+    <t>T051</t>
+  </si>
+  <si>
+    <t>T052</t>
+  </si>
+  <si>
+    <t>T053</t>
+  </si>
+  <si>
+    <t>T054</t>
+  </si>
+  <si>
+    <t>T055</t>
+  </si>
+  <si>
+    <t>T056</t>
+  </si>
+  <si>
+    <t>Story 8 - Sprint 1</t>
+  </si>
+  <si>
+    <t>Story 9 - Sprint 1</t>
+  </si>
+  <si>
+    <t>Story 10 - Sprint 1</t>
+  </si>
+  <si>
+    <t>Story 11 - Sprint 1</t>
+  </si>
+  <si>
+    <t>Story 12 - Sprint 1</t>
+  </si>
+  <si>
+    <t>Story 14 - Sprint 1</t>
+  </si>
+  <si>
+    <t>Story 4 - Sprint 2</t>
+  </si>
+  <si>
+    <t>Create page within the dashboard for displaying a list of shipments - with pagination plugin.</t>
+  </si>
+  <si>
+    <t>Write code to connect to the database and output the shipment results in a list.</t>
+  </si>
+  <si>
+    <t>Create a page within the dashboard for displaying all the data related to a single shipment (individual shipment page)</t>
+  </si>
+  <si>
+    <t>Create a page within the dashboard to give the user the option to update the status.</t>
+  </si>
+  <si>
+    <t>Write code to modify the shipment status in the database</t>
+  </si>
+  <si>
+    <t>Create dashboard portal for employees</t>
+  </si>
+  <si>
+    <t>Create page within the dashboard for displaying a list of contacts.</t>
+  </si>
+  <si>
+    <t>Create customers table within the database to store their details.</t>
+  </si>
+  <si>
+    <t>Write code to connect to the database and output the results in a list.</t>
+  </si>
+  <si>
+    <t>Use plugin to create pagination for data</t>
+  </si>
+  <si>
+    <t>Create page within the dashboard for displaying all the data related to a single customer</t>
+  </si>
+  <si>
+    <t>Story 1 - Sprint 2</t>
+  </si>
+  <si>
+    <t>Story 5 - Sprint 2</t>
+  </si>
+  <si>
+    <t>Create page within the dashboard for displaying a list of payments - with pagination plugin.</t>
+  </si>
+  <si>
+    <t>Write code to connect to the database and output the payment results in a list.</t>
+  </si>
+  <si>
+    <t>Create a page within the dashboard to give the user the option to update the status of the payment.</t>
+  </si>
+  <si>
+    <t>Write code to modify the payment status in the database</t>
+  </si>
+  <si>
+    <t>T057</t>
+  </si>
+  <si>
+    <t>T058</t>
+  </si>
+  <si>
+    <t>T059</t>
+  </si>
+  <si>
+    <t>T060</t>
+  </si>
+  <si>
+    <t>T061</t>
+  </si>
+  <si>
+    <t>T062</t>
+  </si>
+  <si>
+    <t>T063</t>
+  </si>
+  <si>
+    <t>T064</t>
+  </si>
+  <si>
+    <t>T065</t>
+  </si>
+  <si>
+    <t>T066</t>
+  </si>
+  <si>
+    <t>T067</t>
+  </si>
+  <si>
+    <t>T068</t>
+  </si>
+  <si>
+    <t>T069</t>
+  </si>
+  <si>
+    <t>T070</t>
+  </si>
+  <si>
+    <t>T071</t>
+  </si>
+  <si>
+    <t>T072</t>
+  </si>
+  <si>
+    <t>T073</t>
+  </si>
+  <si>
+    <t>T074</t>
+  </si>
+  <si>
+    <t>T075</t>
+  </si>
+  <si>
+    <t>Story 18 - Sprint 2</t>
+  </si>
+  <si>
+    <t>Create page within the dashboard for displaying a list of all pending pickups and package drop offs - with pagination plugin (table sorted by postcode).</t>
+  </si>
+  <si>
+    <t>Create a page to assign certain deliveries or pickups to a single driver.</t>
+  </si>
+  <si>
+    <t>Write code to modify the shipment data in the database to reflect the employee’s id.</t>
+  </si>
+  <si>
+    <t>Write code to send an automatic notification to the driver that they have been assigned pickups or deliveries.</t>
+  </si>
+  <si>
+    <t>Story 19 - Sprint 3</t>
+  </si>
+  <si>
+    <t>Create expenses page where the coordinator can view all expenses.</t>
+  </si>
+  <si>
+    <t>Create a table within the database which stores expenses</t>
+  </si>
+  <si>
+    <t>Create a php connection on the expenses page to output all of the expenses within the expenses table.</t>
+  </si>
+  <si>
+    <t>Create a page with a form where the coordinator can add expenses incurred by employees.</t>
+  </si>
+  <si>
+    <t>Create a page that submits data that is entered into the form to the database, which redirects back to the expenses page.</t>
+  </si>
+  <si>
+    <t>Story 20 - Sprint 3</t>
+  </si>
+  <si>
+    <t>Create page within the dashboard with forms for a pickup request.</t>
+  </si>
+  <si>
+    <t>Create table in the database and write code to connect and store the information entered into the form.</t>
+  </si>
+  <si>
+    <t>Create page to display a list of existing requests</t>
+  </si>
+  <si>
+    <t>T076</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d\-mmm"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -248,16 +714,28 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -265,14 +743,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,9 +927,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nb-NO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -385,7 +953,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1400" strike="noStrike" spc="-1">
+              <a:rPr lang="en-AU" sz="1400" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -485,6 +1053,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AC52-49A9-8B8A-A251FB5BC50B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -562,6 +1135,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AC52-49A9-8B8A-A251FB5BC50B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -609,7 +1187,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-AU" sz="1000" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -703,7 +1281,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-AU" sz="1000" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -795,9 +1373,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nb-NO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -821,7 +1399,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1400" strike="noStrike" spc="-1">
+              <a:rPr lang="en-AU" sz="1400" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -921,6 +1499,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A24-40D2-AC2E-F6B7DF611A41}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -998,6 +1581,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0A24-40D2-AC2E-F6B7DF611A41}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1045,7 +1633,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-AU" sz="1000" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1139,7 +1727,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-AU" sz="1000" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1231,9 +1819,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nb-NO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1257,7 +1845,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1400" strike="noStrike" spc="-1">
+              <a:rPr lang="en-AU" sz="1400" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1357,6 +1945,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-67E3-4BAF-B5FB-9D5F5BC0A62F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1434,6 +2027,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-67E3-4BAF-B5FB-9D5F5BC0A62F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1481,7 +2079,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-AU" sz="1000" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1575,7 +2173,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-AU" sz="1000" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1667,9 +2265,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nb-NO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1709,7 +2307,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1761,28 +2358,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1794,6 +2391,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B6E-43D7-968A-DDA46B3EBB10}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1871,6 +2473,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9B6E-43D7-968A-DDA46B3EBB10}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1996,7 +2603,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2045,7 +2651,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 4"/>
+        <xdr:cNvPr id="2" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2080,7 +2692,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2115,7 +2733,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2150,7 +2774,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2169,7 +2799,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2244,6 +2874,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2279,6 +2926,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2434,10 +3098,10 @@
   <dimension ref="A2:M12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="A5" sqref="A5:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.625"/>
     <col min="2" max="11" width="8.5"/>
@@ -2855,7 +3519,7 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.625"/>
     <col min="2" max="1025" width="8.5"/>
@@ -3174,10 +3838,10 @@
   <dimension ref="A3:P12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5"/>
     <col min="2" max="1025" width="8.5"/>
@@ -3601,13 +4265,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5"/>
+    <col min="1" max="1" width="22.125" customWidth="1"/>
+    <col min="2" max="1025" width="8.5"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -3837,7 +4502,7 @@
       </c>
       <c r="B8">
         <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8</f>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -3861,17 +4526,17 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
         <f>SUM(C8:L8)</f>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="P8" t="s">
         <v>67</v>
@@ -3883,39 +4548,39 @@
       </c>
       <c r="B9">
         <f>SUM(B4:B8)</f>
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:L9" si="0">B9-SUM(C4:C8)</f>
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
@@ -3979,4 +4644,1667 @@
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="3" max="3" width="75.625" customWidth="1"/>
+    <col min="4" max="4" width="6.125" customWidth="1"/>
+    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="6" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="18.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="3"/>
+      <c r="H3">
+        <f>SUM(F4:F12)</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1.5</v>
+      </c>
+      <c r="H4">
+        <f>H3-G4</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f>H4-G5</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H12" si="0">H5-G6</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9">
+        <v>1.5</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11">
+        <v>1.5</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26"/>
+      <c r="B17" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="10">
+        <v>1</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1</v>
+      </c>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18">
+        <v>1.5</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+      <c r="G23" s="10">
+        <v>1</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="M24" s="3"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="F27">
+        <v>0.5</v>
+      </c>
+      <c r="G27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="22"/>
+      <c r="B28" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="19"/>
+      <c r="F28" s="10">
+        <v>2</v>
+      </c>
+      <c r="G28" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29">
+        <v>1.5</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="22"/>
+      <c r="B35" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="19"/>
+      <c r="F35" s="10">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10">
+        <v>1</v>
+      </c>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="F36">
+        <v>1.5</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="20"/>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="20"/>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E39" s="20"/>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="20"/>
+      <c r="F40">
+        <v>2.5</v>
+      </c>
+      <c r="G40">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="22"/>
+      <c r="B41" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E41" s="19"/>
+      <c r="F41" s="10">
+        <v>1</v>
+      </c>
+      <c r="G41" s="10">
+        <v>1</v>
+      </c>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42">
+        <v>3</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="21"/>
+      <c r="B44" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" t="s">
+        <v>177</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="B45" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" t="s">
+        <v>178</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45">
+        <v>0.5</v>
+      </c>
+      <c r="G45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" t="s">
+        <v>179</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="21"/>
+      <c r="B47" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+      <c r="B48" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" t="s">
+        <v>181</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="22"/>
+      <c r="B49" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="17"/>
+      <c r="F49" s="10">
+        <v>1</v>
+      </c>
+      <c r="G49" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H49" s="10"/>
+    </row>
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
+        <v>171</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" t="s">
+        <v>121</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52">
+        <v>0.5</v>
+      </c>
+      <c r="G52">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+      <c r="B53" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+      <c r="B54" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" t="s">
+        <v>174</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
+      <c r="B55" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C55" t="s">
+        <v>175</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55">
+        <v>0.5</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="22"/>
+      <c r="B56" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E56" s="17"/>
+      <c r="F56" s="10">
+        <v>1</v>
+      </c>
+      <c r="G56" s="10">
+        <v>1</v>
+      </c>
+      <c r="H56" s="10"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C57" t="s">
+        <v>184</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="G57">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E58" s="5"/>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+      <c r="B59" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" t="s">
+        <v>185</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E59" s="5"/>
+      <c r="F59">
+        <v>0.5</v>
+      </c>
+      <c r="G59">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="21"/>
+      <c r="B60" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C60" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+      <c r="B61" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C61" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61">
+        <v>0.5</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="22"/>
+      <c r="B62" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E62" s="17"/>
+      <c r="F62" s="10">
+        <v>1</v>
+      </c>
+      <c r="G62" s="10">
+        <v>1</v>
+      </c>
+      <c r="H62" s="10"/>
+    </row>
+    <row r="63" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="G63">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+      <c r="B64" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" s="5"/>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="21"/>
+      <c r="B65" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" t="s">
+        <v>209</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E65" s="5"/>
+      <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="G65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+      <c r="B66" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" t="s">
+        <v>210</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E66" s="5"/>
+      <c r="F66">
+        <v>0.5</v>
+      </c>
+      <c r="G66">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="22"/>
+      <c r="B67" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" s="17"/>
+      <c r="F67" s="10">
+        <v>1</v>
+      </c>
+      <c r="G67" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C68" t="s">
+        <v>121</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E68" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="21"/>
+      <c r="B69" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C69" t="s">
+        <v>213</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E69" s="16"/>
+      <c r="F69">
+        <v>1.5</v>
+      </c>
+      <c r="G69">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="21"/>
+      <c r="B70" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C70" t="s">
+        <v>214</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E70" s="16"/>
+      <c r="F70">
+        <v>0.5</v>
+      </c>
+      <c r="G70">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="21"/>
+      <c r="B71" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C71" t="s">
+        <v>215</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E71" s="16"/>
+      <c r="F71">
+        <v>0.5</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="21"/>
+      <c r="B72" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C72" t="s">
+        <v>216</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E72" s="16"/>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="G72">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="21"/>
+      <c r="B73" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C73" t="s">
+        <v>217</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E73" s="16"/>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="22"/>
+      <c r="B74" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E74" s="17"/>
+      <c r="F74" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G74" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H74" s="10"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C75" t="s">
+        <v>219</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E75" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F75">
+        <v>2</v>
+      </c>
+      <c r="G75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="21"/>
+      <c r="B76" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C76" t="s">
+        <v>220</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E76" s="16"/>
+      <c r="F76">
+        <v>2</v>
+      </c>
+      <c r="G76">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="21"/>
+      <c r="B77" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C77" t="s">
+        <v>221</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E77" s="16"/>
+      <c r="F77">
+        <v>1.5</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+      <c r="B78" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C78" t="s">
+        <v>121</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E78" s="16"/>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="22"/>
+      <c r="B79" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E79" s="17"/>
+      <c r="F79" s="10">
+        <v>1</v>
+      </c>
+      <c r="G79" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H79" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="E75:E79"/>
+    <mergeCell ref="A75:A79"/>
+    <mergeCell ref="E63:E67"/>
+    <mergeCell ref="E57:E62"/>
+    <mergeCell ref="E50:E56"/>
+    <mergeCell ref="E42:E49"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="E68:E74"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="E29:E35"/>
+    <mergeCell ref="E36:E41"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="E4:E12"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="E18:E23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>